<commit_message>
Update with data 4/1/23
</commit_message>
<xml_diff>
--- a/data/raw_data/manual_check_water_depth.xlsx
+++ b/data/raw_data/manual_check_water_depth.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Anne-Marie\KUL\Master\Masterthesis\github repository\data\raw_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{660451B0-87C8-4665-BA0B-88635ED161F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{036C13A5-D984-452C-9630-3D79184E7510}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{BF0455CF-DD72-4E4E-81CB-493DB7D8E4C4}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="44">
   <si>
     <t>SerialNumber</t>
   </si>
@@ -264,7 +264,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -301,6 +301,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -608,7 +611,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -616,10 +619,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2165085E-C73E-4745-9CF5-000463140AFD}">
-  <dimension ref="A1:F44"/>
+  <dimension ref="A1:F49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="A44" sqref="A44:XFD44"/>
+    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
+      <selection activeCell="F48" sqref="F48:F49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -849,26 +852,26 @@
         <v>20.170000000000002</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="15" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>26</v>
-      </c>
-      <c r="B11" s="8" t="s">
-        <v>9</v>
+        <v>22</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>3</v>
       </c>
       <c r="C11" s="6">
-        <v>44775.743055555555</v>
+        <v>44930.597222222219</v>
       </c>
       <c r="D11" s="10">
-        <v>2.1</v>
+        <v>1.17</v>
       </c>
       <c r="E11" s="10">
-        <f>$D11-'well info'!$C$3</f>
-        <v>1.6700000000000002</v>
+        <f>$D11-'well info'!$C$2</f>
+        <v>0.60999999999999988</v>
       </c>
       <c r="F11" s="10">
-        <f>'well info'!$E$3-$E11</f>
-        <v>18.829999999999998</v>
+        <f>'well info'!$E$2-$E11</f>
+        <v>20.69</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="15" x14ac:dyDescent="0.3">
@@ -879,18 +882,18 @@
         <v>9</v>
       </c>
       <c r="C12" s="6">
-        <v>44791.402777777781</v>
+        <v>44775.743055555555</v>
       </c>
       <c r="D12" s="10">
-        <v>2.0499999999999998</v>
+        <v>2.1</v>
       </c>
       <c r="E12" s="10">
         <f>$D12-'well info'!$C$3</f>
-        <v>1.6199999999999999</v>
+        <v>1.6700000000000002</v>
       </c>
       <c r="F12" s="10">
         <f>'well info'!$E$3-$E12</f>
-        <v>18.88</v>
+        <v>18.829999999999998</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="15" x14ac:dyDescent="0.3">
@@ -901,18 +904,18 @@
         <v>9</v>
       </c>
       <c r="C13" s="6">
-        <v>44813.4375</v>
+        <v>44791.402777777781</v>
       </c>
       <c r="D13" s="10">
-        <v>2.1</v>
+        <v>2.0499999999999998</v>
       </c>
       <c r="E13" s="10">
         <f>$D13-'well info'!$C$3</f>
-        <v>1.6700000000000002</v>
+        <v>1.6199999999999999</v>
       </c>
       <c r="F13" s="10">
         <f>'well info'!$E$3-$E13</f>
-        <v>18.829999999999998</v>
+        <v>18.88</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="15" x14ac:dyDescent="0.3">
@@ -923,18 +926,18 @@
         <v>9</v>
       </c>
       <c r="C14" s="6">
-        <v>44818.625</v>
+        <v>44813.4375</v>
       </c>
       <c r="D14" s="10">
-        <v>2.08</v>
+        <v>2.1</v>
       </c>
       <c r="E14" s="10">
         <f>$D14-'well info'!$C$3</f>
-        <v>1.6500000000000001</v>
+        <v>1.6700000000000002</v>
       </c>
       <c r="F14" s="10">
         <f>'well info'!$E$3-$E14</f>
-        <v>18.850000000000001</v>
+        <v>18.829999999999998</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="15" x14ac:dyDescent="0.3">
@@ -945,18 +948,18 @@
         <v>9</v>
       </c>
       <c r="C15" s="6">
-        <v>44824.427083333336</v>
+        <v>44818.625</v>
       </c>
       <c r="D15" s="10">
-        <v>2</v>
+        <v>2.08</v>
       </c>
       <c r="E15" s="10">
         <f>$D15-'well info'!$C$3</f>
-        <v>1.57</v>
+        <v>1.6500000000000001</v>
       </c>
       <c r="F15" s="10">
         <f>'well info'!$E$3-$E15</f>
-        <v>18.93</v>
+        <v>18.850000000000001</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="15" x14ac:dyDescent="0.3">
@@ -967,18 +970,18 @@
         <v>9</v>
       </c>
       <c r="C16" s="6">
-        <v>44851.65625</v>
+        <v>44824.427083333336</v>
       </c>
       <c r="D16" s="10">
-        <v>1.89</v>
+        <v>2</v>
       </c>
       <c r="E16" s="10">
         <f>$D16-'well info'!$C$3</f>
-        <v>1.46</v>
+        <v>1.57</v>
       </c>
       <c r="F16" s="10">
         <f>'well info'!$E$3-$E16</f>
-        <v>19.04</v>
+        <v>18.93</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="15" x14ac:dyDescent="0.3">
@@ -989,18 +992,18 @@
         <v>9</v>
       </c>
       <c r="C17" s="6">
-        <v>44886.625</v>
+        <v>44851.65625</v>
       </c>
       <c r="D17" s="10">
-        <v>1.68</v>
+        <v>1.89</v>
       </c>
       <c r="E17" s="10">
         <f>$D17-'well info'!$C$3</f>
-        <v>1.25</v>
+        <v>1.46</v>
       </c>
       <c r="F17" s="10">
         <f>'well info'!$E$3-$E17</f>
-        <v>19.25</v>
+        <v>19.04</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="15" x14ac:dyDescent="0.3">
@@ -1011,18 +1014,18 @@
         <v>9</v>
       </c>
       <c r="C18" s="6">
-        <v>44894.625</v>
+        <v>44886.625</v>
       </c>
       <c r="D18" s="10">
-        <v>1.4</v>
+        <v>1.68</v>
       </c>
       <c r="E18" s="10">
         <f>$D18-'well info'!$C$3</f>
-        <v>0.97</v>
+        <v>1.25</v>
       </c>
       <c r="F18" s="10">
         <f>'well info'!$E$3-$E18</f>
-        <v>19.53</v>
+        <v>19.25</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="15" x14ac:dyDescent="0.3">
@@ -1033,62 +1036,62 @@
         <v>9</v>
       </c>
       <c r="C19" s="6">
-        <v>44915.416666666664</v>
+        <v>44894.625</v>
       </c>
       <c r="D19" s="10">
-        <v>1.6</v>
+        <v>1.4</v>
       </c>
       <c r="E19" s="10">
         <f>$D19-'well info'!$C$3</f>
-        <v>1.1700000000000002</v>
+        <v>0.97</v>
       </c>
       <c r="F19" s="10">
         <f>'well info'!$E$3-$E19</f>
-        <v>19.329999999999998</v>
+        <v>19.53</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="15" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C20" s="6">
-        <v>44775.510416666664</v>
+        <v>44915.416666666664</v>
       </c>
       <c r="D20" s="10">
-        <v>2.15</v>
+        <v>1.6</v>
       </c>
       <c r="E20" s="10">
-        <f>$D20-'well info'!$C$4</f>
-        <v>1.52</v>
+        <f>$D20-'well info'!$C$3</f>
+        <v>1.1700000000000002</v>
       </c>
       <c r="F20" s="10">
-        <f>'well info'!$E$4-$E20</f>
-        <v>18.18</v>
+        <f>'well info'!$E$3-$E20</f>
+        <v>19.329999999999998</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="15" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C21" s="6">
-        <v>44791.404166666667</v>
+        <v>44930.597222222219</v>
       </c>
       <c r="D21" s="10">
-        <v>1.94</v>
+        <v>0.98</v>
       </c>
       <c r="E21" s="10">
-        <f>$D21-'well info'!$C$4</f>
-        <v>1.31</v>
+        <f>$D21-'well info'!$C$3</f>
+        <v>0.55000000000000004</v>
       </c>
       <c r="F21" s="10">
-        <f>'well info'!$E$4-$E21</f>
-        <v>18.39</v>
+        <f>'well info'!$E$3-$E21</f>
+        <v>19.95</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="15" x14ac:dyDescent="0.3">
@@ -1099,18 +1102,18 @@
         <v>7</v>
       </c>
       <c r="C22" s="6">
-        <v>44813.44027777778</v>
+        <v>44775.510416666664</v>
       </c>
       <c r="D22" s="10">
-        <v>1.94</v>
+        <v>2.15</v>
       </c>
       <c r="E22" s="10">
-        <f>D22-'well info'!$C$4</f>
-        <v>1.31</v>
+        <f>$D22-'well info'!$C$4</f>
+        <v>1.52</v>
       </c>
       <c r="F22" s="10">
         <f>'well info'!$E$4-$E22</f>
-        <v>18.39</v>
+        <v>18.18</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="15" x14ac:dyDescent="0.3">
@@ -1121,18 +1124,18 @@
         <v>7</v>
       </c>
       <c r="C23" s="6">
-        <v>44818.607638888891</v>
+        <v>44791.404166666667</v>
       </c>
       <c r="D23" s="10">
-        <v>1.92</v>
+        <v>1.94</v>
       </c>
       <c r="E23" s="10">
-        <f>D23-'well info'!$C$4</f>
-        <v>1.29</v>
+        <f>$D23-'well info'!$C$4</f>
+        <v>1.31</v>
       </c>
       <c r="F23" s="10">
         <f>'well info'!$E$4-$E23</f>
-        <v>18.41</v>
+        <v>18.39</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="15" x14ac:dyDescent="0.3">
@@ -1143,18 +1146,18 @@
         <v>7</v>
       </c>
       <c r="C24" s="6">
-        <v>44824.430555555555</v>
+        <v>44813.44027777778</v>
       </c>
       <c r="D24" s="10">
-        <v>1.88</v>
+        <v>1.94</v>
       </c>
       <c r="E24" s="10">
         <f>D24-'well info'!$C$4</f>
-        <v>1.25</v>
+        <v>1.31</v>
       </c>
       <c r="F24" s="10">
         <f>'well info'!$E$4-$E24</f>
-        <v>18.45</v>
+        <v>18.39</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="15" x14ac:dyDescent="0.3">
@@ -1165,18 +1168,18 @@
         <v>7</v>
       </c>
       <c r="C25" s="6">
-        <v>44851.65625</v>
+        <v>44818.607638888891</v>
       </c>
       <c r="D25" s="10">
-        <v>1.76</v>
+        <v>1.92</v>
       </c>
       <c r="E25" s="10">
         <f>D25-'well info'!$C$4</f>
-        <v>1.1299999999999999</v>
+        <v>1.29</v>
       </c>
       <c r="F25" s="10">
         <f>'well info'!$E$4-$E25</f>
-        <v>18.57</v>
+        <v>18.41</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="15" x14ac:dyDescent="0.3">
@@ -1187,18 +1190,18 @@
         <v>7</v>
       </c>
       <c r="C26" s="6">
-        <v>44886.625</v>
+        <v>44824.430555555555</v>
       </c>
       <c r="D26" s="10">
-        <v>1.43</v>
+        <v>1.88</v>
       </c>
       <c r="E26" s="10">
         <f>D26-'well info'!$C$4</f>
-        <v>0.79999999999999993</v>
+        <v>1.25</v>
       </c>
       <c r="F26" s="10">
         <f>'well info'!$E$4-$E26</f>
-        <v>18.899999999999999</v>
+        <v>18.45</v>
       </c>
     </row>
     <row r="27" spans="1:6" ht="15" x14ac:dyDescent="0.3">
@@ -1209,18 +1212,18 @@
         <v>7</v>
       </c>
       <c r="C27" s="6">
-        <v>44894.625</v>
+        <v>44851.65625</v>
       </c>
       <c r="D27" s="10">
-        <v>1.25</v>
+        <v>1.76</v>
       </c>
       <c r="E27" s="10">
         <f>D27-'well info'!$C$4</f>
-        <v>0.62</v>
+        <v>1.1299999999999999</v>
       </c>
       <c r="F27" s="10">
         <f>'well info'!$E$4-$E27</f>
-        <v>19.079999999999998</v>
+        <v>18.57</v>
       </c>
     </row>
     <row r="28" spans="1:6" ht="15" x14ac:dyDescent="0.3">
@@ -1231,84 +1234,84 @@
         <v>7</v>
       </c>
       <c r="C28" s="6">
-        <v>44915.416666666664</v>
+        <v>44886.625</v>
       </c>
       <c r="D28" s="10">
-        <v>1.37</v>
+        <v>1.43</v>
       </c>
       <c r="E28" s="10">
         <f>D28-'well info'!$C$4</f>
-        <v>0.7400000000000001</v>
+        <v>0.79999999999999993</v>
       </c>
       <c r="F28" s="10">
         <f>'well info'!$E$4-$E28</f>
+        <v>18.899999999999999</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="15" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>24</v>
+      </c>
+      <c r="B29" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C29" s="6">
+        <v>44894.625</v>
+      </c>
+      <c r="D29" s="10">
+        <v>1.25</v>
+      </c>
+      <c r="E29" s="10">
+        <f>D29-'well info'!$C$4</f>
+        <v>0.62</v>
+      </c>
+      <c r="F29" s="10">
+        <f>'well info'!$E$4-$E29</f>
+        <v>19.079999999999998</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="15" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>24</v>
+      </c>
+      <c r="B30" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C30" s="6">
+        <v>44915.416666666664</v>
+      </c>
+      <c r="D30" s="10">
+        <v>1.37</v>
+      </c>
+      <c r="E30" s="10">
+        <f>D30-'well info'!$C$4</f>
+        <v>0.7400000000000001</v>
+      </c>
+      <c r="F30" s="10">
+        <f>'well info'!$E$4-$E30</f>
         <v>18.96</v>
       </c>
     </row>
-    <row r="29" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A29" t="s">
-        <v>23</v>
-      </c>
-      <c r="B29" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C29" s="6">
-        <v>44775.552083333336</v>
-      </c>
-      <c r="D29" s="10">
-        <v>2.83</v>
-      </c>
-      <c r="E29" s="10">
-        <f>$D29-'well info'!$C$5</f>
-        <v>2.15</v>
-      </c>
-      <c r="F29" s="10">
-        <f>'well info'!$E$5-$E29</f>
-        <v>18.75</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A30" t="s">
-        <v>23</v>
-      </c>
-      <c r="B30" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C30" s="6">
-        <v>44791.406944444447</v>
-      </c>
-      <c r="D30" s="10">
-        <v>2.71</v>
-      </c>
-      <c r="E30" s="10">
-        <f>$D30-'well info'!$C$5</f>
-        <v>2.0299999999999998</v>
-      </c>
-      <c r="F30" s="10">
-        <f>'well info'!$E$5-$E30</f>
-        <v>18.869999999999997</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:6" ht="15" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>23</v>
-      </c>
-      <c r="B31" s="3" t="s">
-        <v>6</v>
+        <v>24</v>
+      </c>
+      <c r="B31" s="8" t="s">
+        <v>7</v>
       </c>
       <c r="C31" s="6">
-        <v>44813.447916666664</v>
+        <v>44930.597222222219</v>
       </c>
       <c r="D31" s="10">
-        <v>2.89</v>
+        <v>1.08</v>
       </c>
       <c r="E31" s="10">
-        <f>$D31-'well info'!$C$5</f>
-        <v>2.21</v>
+        <f>D31-'well info'!$C$4</f>
+        <v>0.45000000000000007</v>
       </c>
       <c r="F31" s="10">
-        <f>'well info'!$E$5-$E31</f>
-        <v>18.689999999999998</v>
+        <f>'well info'!$E$4-$E31</f>
+        <v>19.25</v>
       </c>
     </row>
     <row r="32" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
@@ -1319,18 +1322,18 @@
         <v>6</v>
       </c>
       <c r="C32" s="6">
-        <v>44818.607638888891</v>
+        <v>44775.552083333336</v>
       </c>
       <c r="D32" s="10">
-        <v>2.77</v>
+        <v>2.83</v>
       </c>
       <c r="E32" s="10">
         <f>$D32-'well info'!$C$5</f>
-        <v>2.09</v>
+        <v>2.15</v>
       </c>
       <c r="F32" s="10">
         <f>'well info'!$E$5-$E32</f>
-        <v>18.809999999999999</v>
+        <v>18.75</v>
       </c>
     </row>
     <row r="33" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
@@ -1341,18 +1344,18 @@
         <v>6</v>
       </c>
       <c r="C33" s="6">
-        <v>44824.431944444441</v>
+        <v>44791.406944444447</v>
       </c>
       <c r="D33" s="10">
-        <v>2.68</v>
+        <v>2.71</v>
       </c>
       <c r="E33" s="10">
         <f>$D33-'well info'!$C$5</f>
-        <v>2</v>
+        <v>2.0299999999999998</v>
       </c>
       <c r="F33" s="10">
         <f>'well info'!$E$5-$E33</f>
-        <v>18.899999999999999</v>
+        <v>18.869999999999997</v>
       </c>
     </row>
     <row r="34" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
@@ -1363,18 +1366,18 @@
         <v>6</v>
       </c>
       <c r="C34" s="6">
-        <v>44886.618055555555</v>
+        <v>44813.447916666664</v>
       </c>
       <c r="D34" s="10">
-        <v>2.23</v>
+        <v>2.89</v>
       </c>
       <c r="E34" s="10">
         <f>$D34-'well info'!$C$5</f>
-        <v>1.5499999999999998</v>
+        <v>2.21</v>
       </c>
       <c r="F34" s="10">
         <f>'well info'!$E$5-$E34</f>
-        <v>19.349999999999998</v>
+        <v>18.689999999999998</v>
       </c>
     </row>
     <row r="35" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
@@ -1385,18 +1388,18 @@
         <v>6</v>
       </c>
       <c r="C35" s="6">
-        <v>44894.625</v>
+        <v>44818.607638888891</v>
       </c>
       <c r="D35" s="10">
-        <v>1.81</v>
+        <v>2.77</v>
       </c>
       <c r="E35" s="10">
         <f>$D35-'well info'!$C$5</f>
-        <v>1.1299999999999999</v>
+        <v>2.09</v>
       </c>
       <c r="F35" s="10">
         <f>'well info'!$E$5-$E35</f>
-        <v>19.77</v>
+        <v>18.809999999999999</v>
       </c>
     </row>
     <row r="36" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
@@ -1407,106 +1410,106 @@
         <v>6</v>
       </c>
       <c r="C36" s="6">
-        <v>44915.416666666664</v>
+        <v>44824.431944444441</v>
       </c>
       <c r="D36" s="10">
-        <v>2.11</v>
+        <v>2.68</v>
       </c>
       <c r="E36" s="10">
         <f>$D36-'well info'!$C$5</f>
-        <v>1.4299999999999997</v>
+        <v>2</v>
       </c>
       <c r="F36" s="10">
         <f>'well info'!$E$5-$E36</f>
+        <v>18.899999999999999</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>23</v>
+      </c>
+      <c r="B37" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C37" s="6">
+        <v>44886.618055555555</v>
+      </c>
+      <c r="D37" s="10">
+        <v>2.23</v>
+      </c>
+      <c r="E37" s="10">
+        <f>$D37-'well info'!$C$5</f>
+        <v>1.5499999999999998</v>
+      </c>
+      <c r="F37" s="10">
+        <f>'well info'!$E$5-$E37</f>
+        <v>19.349999999999998</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>23</v>
+      </c>
+      <c r="B38" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C38" s="6">
+        <v>44894.625</v>
+      </c>
+      <c r="D38" s="10">
+        <v>1.81</v>
+      </c>
+      <c r="E38" s="10">
+        <f>$D38-'well info'!$C$5</f>
+        <v>1.1299999999999999</v>
+      </c>
+      <c r="F38" s="10">
+        <f>'well info'!$E$5-$E38</f>
+        <v>19.77</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>23</v>
+      </c>
+      <c r="B39" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C39" s="6">
+        <v>44915.416666666664</v>
+      </c>
+      <c r="D39" s="10">
+        <v>2.11</v>
+      </c>
+      <c r="E39" s="10">
+        <f>$D39-'well info'!$C$5</f>
+        <v>1.4299999999999997</v>
+      </c>
+      <c r="F39" s="10">
+        <f>'well info'!$E$5-$E39</f>
         <v>19.47</v>
       </c>
     </row>
-    <row r="37" spans="1:6" ht="15" x14ac:dyDescent="0.3">
-      <c r="A37" t="s">
-        <v>25</v>
-      </c>
-      <c r="B37" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="C37" s="6">
-        <v>44775.552083333336</v>
-      </c>
-      <c r="D37" s="10">
-        <v>99</v>
-      </c>
-      <c r="E37" s="10">
-        <f>$D37-'well info'!$C$6</f>
-        <v>98.3</v>
-      </c>
-      <c r="F37" s="10">
-        <f>'well info'!$E$2-$E37</f>
-        <v>-77</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" ht="15" x14ac:dyDescent="0.3">
-      <c r="A38" t="s">
-        <v>25</v>
-      </c>
-      <c r="B38" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="C38" s="6">
-        <v>44791.408333333333</v>
-      </c>
-      <c r="D38" s="10">
-        <v>99</v>
-      </c>
-      <c r="E38" s="10">
-        <f>$D38-'well info'!$C$6</f>
-        <v>98.3</v>
-      </c>
-      <c r="F38" s="10">
-        <f>'well info'!$E$2-$E38</f>
-        <v>-77</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" ht="15" x14ac:dyDescent="0.3">
-      <c r="A39" t="s">
-        <v>25</v>
-      </c>
-      <c r="B39" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="C39" s="6">
-        <v>44813.458333333336</v>
-      </c>
-      <c r="D39" s="10">
-        <v>99</v>
-      </c>
-      <c r="E39" s="10">
-        <f>$D39-'well info'!$C$6</f>
-        <v>98.3</v>
-      </c>
-      <c r="F39" s="10">
-        <f>'well info'!$E$2-$E39</f>
-        <v>-77</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" ht="15" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>25</v>
-      </c>
-      <c r="B40" s="8" t="s">
-        <v>8</v>
+        <v>23</v>
+      </c>
+      <c r="B40" s="3" t="s">
+        <v>6</v>
       </c>
       <c r="C40" s="6">
-        <v>44818.645833333336</v>
+        <v>44930.597222222219</v>
       </c>
       <c r="D40" s="10">
-        <v>99</v>
+        <v>1.2</v>
       </c>
       <c r="E40" s="10">
-        <f>$D40-'well info'!$C$6</f>
-        <v>98.3</v>
+        <f>$D40-'well info'!$C$5</f>
+        <v>0.51999999999999991</v>
       </c>
       <c r="F40" s="10">
-        <f>'well info'!$E$2-$E40</f>
-        <v>-77</v>
+        <f>'well info'!$E$5-$E40</f>
+        <v>20.38</v>
       </c>
     </row>
     <row r="41" spans="1:6" ht="15" x14ac:dyDescent="0.3">
@@ -1517,7 +1520,7 @@
         <v>8</v>
       </c>
       <c r="C41" s="6">
-        <v>44824.434027777781</v>
+        <v>44775.552083333336</v>
       </c>
       <c r="D41" s="10">
         <v>99</v>
@@ -1535,66 +1538,176 @@
       <c r="A42" t="s">
         <v>25</v>
       </c>
-      <c r="B42" s="12" t="s">
+      <c r="B42" s="8" t="s">
         <v>8</v>
       </c>
       <c r="C42" s="6">
-        <v>44886.597222222219</v>
-      </c>
-      <c r="D42" s="13">
-        <v>4.4800000000000004</v>
+        <v>44791.408333333333</v>
+      </c>
+      <c r="D42" s="10">
+        <v>99</v>
       </c>
       <c r="E42" s="10">
-        <f>$D42-'well info'!$C$8</f>
-        <v>4.2</v>
+        <f>$D42-'well info'!$C$6</f>
+        <v>98.3</v>
       </c>
       <c r="F42" s="10">
-        <f>'well info'!$E$6-$E42</f>
-        <v>18.100000000000001</v>
+        <f>'well info'!$E$2-$E42</f>
+        <v>-77</v>
       </c>
     </row>
     <row r="43" spans="1:6" ht="15" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>25</v>
       </c>
-      <c r="B43" s="12" t="s">
+      <c r="B43" s="8" t="s">
         <v>8</v>
       </c>
       <c r="C43" s="6">
-        <v>44894.625</v>
-      </c>
-      <c r="D43" s="13">
-        <v>2.65</v>
+        <v>44813.458333333336</v>
+      </c>
+      <c r="D43" s="10">
+        <v>99</v>
       </c>
       <c r="E43" s="10">
-        <f>$D43-'well info'!$C$8</f>
-        <v>2.37</v>
+        <f>$D43-'well info'!$C$6</f>
+        <v>98.3</v>
       </c>
       <c r="F43" s="10">
-        <f>'well info'!$E$6-$E43</f>
-        <v>19.93</v>
+        <f>'well info'!$E$2-$E43</f>
+        <v>-77</v>
       </c>
     </row>
     <row r="44" spans="1:6" ht="15" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>25</v>
       </c>
-      <c r="B44" s="12" t="s">
+      <c r="B44" s="8" t="s">
         <v>8</v>
       </c>
       <c r="C44" s="6">
+        <v>44818.645833333336</v>
+      </c>
+      <c r="D44" s="10">
+        <v>99</v>
+      </c>
+      <c r="E44" s="10">
+        <f>$D44-'well info'!$C$6</f>
+        <v>98.3</v>
+      </c>
+      <c r="F44" s="10">
+        <f>'well info'!$E$2-$E44</f>
+        <v>-77</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" ht="15" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>25</v>
+      </c>
+      <c r="B45" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C45" s="6">
+        <v>44824.434027777781</v>
+      </c>
+      <c r="D45" s="10">
+        <v>99</v>
+      </c>
+      <c r="E45" s="10">
+        <f>$D45-'well info'!$C$6</f>
+        <v>98.3</v>
+      </c>
+      <c r="F45" s="10">
+        <f>'well info'!$E$2-$E45</f>
+        <v>-77</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" ht="15" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>25</v>
+      </c>
+      <c r="B46" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="C46" s="6">
+        <v>44886.597222222219</v>
+      </c>
+      <c r="D46" s="13">
+        <v>4.4800000000000004</v>
+      </c>
+      <c r="E46" s="10">
+        <f>$D46-'well info'!$C$8</f>
+        <v>4.2</v>
+      </c>
+      <c r="F46" s="10">
+        <f>'well info'!$E$6-$E46</f>
+        <v>18.100000000000001</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" ht="15" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
+        <v>25</v>
+      </c>
+      <c r="B47" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="C47" s="6">
+        <v>44894.625</v>
+      </c>
+      <c r="D47" s="13">
+        <v>2.65</v>
+      </c>
+      <c r="E47" s="10">
+        <f>$D47-'well info'!$C$8</f>
+        <v>2.37</v>
+      </c>
+      <c r="F47" s="10">
+        <f>'well info'!$E$6-$E47</f>
+        <v>19.93</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" ht="15" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
+        <v>25</v>
+      </c>
+      <c r="B48" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="C48" s="6">
         <v>44915.416666666664</v>
       </c>
-      <c r="D44" s="13">
+      <c r="D48" s="13">
         <v>2.7</v>
       </c>
-      <c r="E44" s="10">
-        <f>$D44-'well info'!$C$8</f>
+      <c r="E48" s="10">
+        <f>$D48-'well info'!$C$8</f>
         <v>2.42</v>
       </c>
-      <c r="F44" s="10">
-        <f>'well info'!$E$6-$E44</f>
+      <c r="F48" s="10">
+        <f>'well info'!$E$6-$E48</f>
         <v>19.880000000000003</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" ht="15" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
+        <v>25</v>
+      </c>
+      <c r="B49" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="C49" s="6">
+        <v>44930.597222222219</v>
+      </c>
+      <c r="D49" s="15">
+        <v>1.38</v>
+      </c>
+      <c r="E49" s="10">
+        <f>$D49-'well info'!$C$8</f>
+        <v>1.0999999999999999</v>
+      </c>
+      <c r="F49" s="10">
+        <f>'well info'!$E$6-$E49</f>
+        <v>21.2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>